<commit_message>
Tippfehler in Textbausteinen korrigiert
</commit_message>
<xml_diff>
--- a/Textbausteine/Textbausteine-Foerderbemerkungen.xlsx
+++ b/Textbausteine/Textbausteine-Foerderbemerkungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pfotenhauer\git\Schild-NRW-GS-Zeugnisse\Textbausteine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA22D38-39BC-431F-BAD1-A8280C675D56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005A762B-20F1-4D51-A56A-709B74131F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30105" yWindow="1035" windowWidth="26985" windowHeight="14610" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>Ein Bericht zum Arbeits- und Sozialverhalten wird dem Zeugnis hinzugefügt, wenn die Versetzungskonferenz dies beschlossen hat und die Schulkonferenz dazu eine einheitliche Vorgehensweise festgelegt hat (§ 49 Absatz 2 Schulgesetzt NRW). Je nach Umfang kann dieser Bericht dem Zeugnis als Anlage hinzugefügt werden.</t>
   </si>
   <si>
-    <t>Wenn nach $ 33 Absatz 3 AO-SF verfahren wird, werden die Noten in das Berichtszeugnis integriert. Es wird darauf hingewiesen, dass sich die Leistungsbewertung mit Noten an den Anforderungen der vorhergehenden Jahrgangsstufe der Grundschule oder der Hauptschule orientiert.</t>
-  </si>
-  <si>
     <t>$Vorname$ nimmt im kommenden Schuljahr am Unterricht der Klasse 10 in einem besonderen Bildungsgang teil, mit dem Ziel, einem dem Hauptschulabschluss (nach Klasse 9) gleichwertigen Abschluss zu erreichen.</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>Die Zugehörigkeit zum Bildungsgang Lernen wurde gemäß § 18 AO-SF durch die Entscheidung des Schulamtes **Wuppertal** der Bezirksregierung **Düsseldorf** vom **tt.mm.jjjj** aufgehoben. Deshalb wird $Vorname§ zukünftig zielgleich im Bildungsgang der allgemeinen Schule unterrichtet. $Vorname$ hat aber weiterhin sonderpädagogischen Förderbedarf im Förderschwerpunkt ****.</t>
+  </si>
+  <si>
+    <t>Wenn nach § 33 Absatz 3 AO-SF verfahren wird, werden die Noten in das Berichtszeugnis integriert. Es wird darauf hingewiesen, dass sich die Leistungsbewertung mit Noten an den Anforderungen der vorhergehenden Jahrgangsstufe der Grundschule oder der Hauptschule orientiert.</t>
   </si>
 </sst>
 </file>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +574,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -590,7 +590,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -598,7 +598,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -606,7 +606,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -614,7 +614,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -662,7 +662,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -686,39 +686,39 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Angepasste Förderfloskeln vom Schulamt Dortmund
</commit_message>
<xml_diff>
--- a/Textbausteine/Textbausteine-Foerderbemerkungen.xlsx
+++ b/Textbausteine/Textbausteine-Foerderbemerkungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pfotenhauer\git\Schild-NRW-GS-Zeugnisse\Textbausteine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne Schüller\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005A762B-20F1-4D51-A56A-709B74131F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F453409-3A99-43A2-9C59-35A23D896300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30105" yWindow="1035" windowWidth="26985" windowHeight="14610" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15750" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Floskelnummer</t>
   </si>
@@ -49,64 +49,79 @@
     <t>Niveau</t>
   </si>
   <si>
-    <t>$Vorname$ wurde im Förderschwerpunkt Lernen sonderpädagogisch gefördert und im Bildungsgang Grundschule unterrichtet.</t>
-  </si>
-  <si>
-    <t>$Vorname$ wurde im Förderschwerpunkt Sprache sonderpädagogisch gefördert und im Bildungsgang Grundschule unterrichtet.</t>
-  </si>
-  <si>
-    <t>$Vorname$ wurde im Förderschwerpunkt geistige Entwicklung sonderpädagogisch gefördert und im Bildungsgang Grundschule unterrichtet.</t>
-  </si>
-  <si>
-    <t>$Vorname$ wurde im Förderschwerpunkt emotionale und soziale Entwicklung sonderpädagogisch gefördert und im Bildungsgang Grundschule unterrichtet.</t>
-  </si>
-  <si>
-    <t>$Vorname$ wurde im Förderschwerpunkt körperliche und motorische Entwicklung sonderpädagogisch gefördert und im Bildungsgang Grundschule unterrichtet.</t>
-  </si>
-  <si>
     <t>$Vorname$ wurde im Förderschwerpunkt Lernen sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Lernen unterrichtet.</t>
   </si>
   <si>
-    <t>$Vorname$ wurde im Förderschwerpunkt Sprache sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Sprache unterrichtet.</t>
-  </si>
-  <si>
-    <t>$Vorname$ wurde im Förderschwerpunkt geistige Entwicklung sonderpädagogisch gefördert und im zieldifferenten Bildungsgang geistige Entwicklung unterrichtet.</t>
-  </si>
-  <si>
-    <t>$Vorname$ wurde im Förderschwerpunkt emotionale und soziale Entwicklung sonderpädagogisch gefördert und im zieldifferenten Bildungsgang emotionale und soziale Entwicklung unterrichtet.</t>
-  </si>
-  <si>
-    <t>$Vorname$ wurde im Förderschwerpunkt körperliche und motorische Entwicklung sonderpädagogisch gefördert und im zieldifferenten Bildungsgang körperliche und motorische Entwicklung unterrichtet.</t>
-  </si>
-  <si>
     <t>$Vorname$ hat gemäß § 18 AO-SF durch die Entscheidung des Schulamtes **Wuppertal** der Bezirksregierung **Düsseldorf** vom **tt.mm.jjjj** keinen Bedarf an sonderpädagogischer Unterstützung mehr.</t>
   </si>
   <si>
     <t>$Vorname$ wechselt gemäß § 18 AO-SF durch die Entscheidung des Schulamtes **Wuppertal** der Bezirksregierung **Düsseldorf** vom **tt.mm.jjjj** den Förderschwerpunkt. &amp;Er%Sie&amp; wird zukünftig im Förderschwerpunkt **** gefördert.</t>
   </si>
   <si>
-    <t>$Vorname$ wechselt gemäß § 18 AO-SF durch die Entscheidung des Schulamtes **Wuppertal** der Bezirksregierung **Düsseldorf** vom **tt.mm.jjjj** im Förderschwerpunkt *** den Bildungsgang. &amp;Er%Sie&amp; wird zukünftig im Bildungsgang **** gefördert.</t>
-  </si>
-  <si>
     <t>Laut Beschluss der Klassenkonferenz vom **tt.mm.jjjj*** besteht gemäß § 17 AO-SF der Bedarf an sonderpädagogischer Unterstützung im Förderschwerpunkt **** mit dem zielgleichen Bildungsgang **** mit dem zieldifferenten **** weiterhin.</t>
   </si>
   <si>
     <t>Ein Bericht zum Arbeits- und Sozialverhalten wird dem Zeugnis hinzugefügt, wenn die Versetzungskonferenz dies beschlossen hat und die Schulkonferenz dazu eine einheitliche Vorgehensweise festgelegt hat (§ 49 Absatz 2 Schulgesetzt NRW). Je nach Umfang kann dieser Bericht dem Zeugnis als Anlage hinzugefügt werden.</t>
   </si>
   <si>
-    <t>$Vorname$ nimmt im kommenden Schuljahr am Unterricht der Klasse 10 in einem besonderen Bildungsgang teil, mit dem Ziel, einem dem Hauptschulabschluss (nach Klasse 9) gleichwertigen Abschluss zu erreichen.</t>
-  </si>
-  <si>
     <t>$Vorname$ hat den Abschluss des Bildungsgangs Lernen erworben.</t>
   </si>
   <si>
     <t>FSP</t>
   </si>
   <si>
-    <t>Die Zugehörigkeit zum Bildungsgang Lernen wurde gemäß § 18 AO-SF durch die Entscheidung des Schulamtes **Wuppertal** der Bezirksregierung **Düsseldorf** vom **tt.mm.jjjj** aufgehoben. Deshalb wird $Vorname§ zukünftig zielgleich im Bildungsgang der allgemeinen Schule unterrichtet. $Vorname$ hat aber weiterhin sonderpädagogischen Förderbedarf im Förderschwerpunkt ****.</t>
-  </si>
-  <si>
     <t>Wenn nach § 33 Absatz 3 AO-SF verfahren wird, werden die Noten in das Berichtszeugnis integriert. Es wird darauf hingewiesen, dass sich die Leistungsbewertung mit Noten an den Anforderungen der vorhergehenden Jahrgangsstufe der Grundschule oder der Hauptschule orientiert.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Sprache sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Lernen unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Emotionale und soziale Entwicklung sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Lernen unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Körperliche und motorische Entwicklung sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Lernen unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Körperliche und motorische Entwicklung sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Geistige Entwicklung unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Geistige Entwicklung sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Geistige Entwicklung unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wechselt gemäß § 17 AO-SF durch die Entscheidung des Schulamtes **Wuppertal** der Bezirksregierung **Düsseldorf** vom **tt.mm.jjjj** im Förderschwerpunkt *** den Bildungsgang. &amp;Er%Sie&amp; wird zukünftig im Bildungsgang **** gefördert.</t>
+  </si>
+  <si>
+    <t>$Vorname$ nimmt im kommenden Schuljahr am Unterricht der Klasse 10 in einem besonderen Bildungsgang teil, mit dem Ziel, einem dem Ersten Schulabschluss gleichwertigen Abschluss zu erreichen.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Hören und Kommunikation sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Lernen unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Hören und Kommunikation sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Geistige Entwicklung unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Sehen sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Lernen unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Sehen sonderpädagogisch gefördert und im zieldifferenten Bildungsgang Geistige Entwicklung unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Sprache sonderpädagogisch gefördert und im Bildungsgang der Grundschule unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Emotionale und soziale Entwicklung sonderpädagogisch gefördert und im Bildungsgang der Grundschule unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Körperliche und motorische Entwicklung sonderpädagogisch gefördert und im Bildungsgang der Grundschule unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Hören und Kommunikation sonderpädagogisch gefördert und im Bildungsgang der Grundschule unterrichtet.</t>
+  </si>
+  <si>
+    <t>$Vorname$ wurde im Förderschwerpunkt Sehen sonderpädagogisch gefördert und im Bildungsgang der Grundschule unterrichtet.</t>
+  </si>
+  <si>
+    <t>Die Zugehörigkeit zum Bildungsgang Lernen wurde gemäß § 18 AO-SF durch die Entscheidung des Schulamtes **Wuppertal** der Bezirksregierung **Düsseldorf** vom **tt.mm.jjjj** aufgehoben. Deshalb wird $Vorname§ zukünftig zielgleich im Bildungsgang der Grundschule unterrichtet. $Vorname$ hat aber weiterhin sonderpädagogischen Förderbedarf im Förderschwerpunkt ****.</t>
   </si>
 </sst>
 </file>
@@ -148,9 +163,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -534,22 +548,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="89.7109375" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="255.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="1023" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,154 +586,181 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>